<commit_message>
api verbunden + draft 3 submit
</commit_message>
<xml_diff>
--- a/-inbox-/services BerlinDE.xlsx
+++ b/-inbox-/services BerlinDE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mghd/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mghd/Cloud/Dropbox/Uni/TU/WiInf, BSc/Modulen/1-SoSe 17/1-Thesis/AlexaImAmt_git/-inbox-/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12000" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10880" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Dienstleistungen" sheetId="1" r:id="rId1"/>
@@ -4245,8 +4245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A682"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="A153" sqref="A153"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>